<commit_message>
Added forms, maps, and route distance calculators
</commit_message>
<xml_diff>
--- a/input/carshare_data_v4.xlsx
+++ b/input/carshare_data_v4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kampw\PycharmProjects\carShareCalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kampw\PycharmProjects\carshare-react\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9814C1F0-E6C0-4B31-9155-9756200520AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EB092-85DA-48B1-B247-78C2D3C530D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED27C62F-BF0F-45ED-B1F2-67EFCF8C1D7C}"/>
   </bookViews>
@@ -721,8 +721,8 @@
   <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A1:A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>